<commit_message>
add sql and dv SESUG project
</commit_message>
<xml_diff>
--- a/SESUG 2023 Visualization/data/SESUG 2023_Visualization Contest_Charlotte Checkers.xlsx
+++ b/SESUG 2023 Visualization/data/SESUG 2023_Visualization Contest_Charlotte Checkers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sasoffice365-my.sharepoint.com/personal/peter_styliadis_sas_com/Documents/github repos/SAS Programming/SESUG 2023 Visualization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{2E5A923E-2D9B-468C-81B7-A040456885AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCD49254-281E-4292-AFBA-441B5FE968A1}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{2E5A923E-2D9B-468C-81B7-A040456885AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8E51AFF-9132-4CE6-A8B6-99C8E43E9C67}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C019BC52-4047-4D97-A61E-D644A0939387}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C019BC52-4047-4D97-A61E-D644A0939387}"/>
   </bookViews>
   <sheets>
     <sheet name="Contest Rules" sheetId="5" r:id="rId1"/>
@@ -3194,9 +3194,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424A353D-7D33-43B1-A8C4-D1AF8BAAAFF4}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3433,23 +3433,6 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E10" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <f>B2*2</f>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <f>SUM(C15:C16)</f>
-        <v>83</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9479,7 +9462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868750C0-AAC3-4EA8-8534-3DC8A9FB5DE6}">
   <dimension ref="A1:M1048574"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18675,7 +18660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C15895-D12D-4089-87E9-AB48C9126EC7}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>